<commit_message>
Team Sports version 0.0.1 - moved from tennis_scheduler to team_sports - changed color scheme to black and gold - unified tab looks between header areas and card areas - completed Teams and Roster screens, added Calendar and Venues screens... - added promises/async dbase operations to prevent racing issues...
</commit_message>
<xml_diff>
--- a/Requirements/Thursday Night Tennis Schedule.2020-2021.xlsx
+++ b/Requirements/Thursday Night Tennis Schedule.2020-2021.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0957328-CB8A-4B18-A88C-C9F49C768CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BA12A5-8D4C-412E-8400-14C41077D027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021 Schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Matches">'2020-2021 Schedule'!$T$12:$AI$14</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="68">
   <si>
     <t>Player</t>
   </si>
@@ -239,6 +240,12 @@
   </si>
   <si>
     <t>Versus</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -918,7 +925,7 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="109">
+  <dxfs count="116">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -931,6 +938,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF6600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF6600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -951,6 +998,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -961,6 +1018,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -971,6 +1038,56 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1041,6 +1158,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1051,6 +1188,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1071,6 +1218,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1081,6 +1238,256 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1091,6 +1498,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1101,6 +1548,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF6600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1111,6 +1578,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1121,6 +1598,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1141,6 +1628,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF6600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1201,6 +1718,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -1221,226 +1748,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1481,16 +1788,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1501,11 +1798,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <color rgb="FF6600FF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1521,66 +1818,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF6600FF"/>
       </font>
       <fill>
@@ -1591,146 +1828,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF6600FF"/>
       </font>
       <fill>
@@ -1741,16 +1838,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF6600FF"/>
       </font>
       <fill>
@@ -1761,43 +1848,57 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF6600FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF6600FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF6600FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2472,55 +2573,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="N18:N37" totalsRowShown="0" headerRowDxfId="108" dataDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="N18:N37" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114">
   <autoFilter ref="N18:N37" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N19:N33">
     <sortCondition ref="N18:N33"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NAME" dataDxfId="106"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NAME" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="T12:AI14" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104" tableBorderDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="T12:AI14" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111" tableBorderDxfId="110">
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Court 3 Week" dataDxfId="102"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Court 3 Match Date" dataDxfId="101">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Court 3 Week" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Court 3 Match Date" dataDxfId="108">
       <calculatedColumnFormula>VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$58,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Court 3 Player 1" dataDxfId="100">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Court 3 Player 1" dataDxfId="107">
       <calculatedColumnFormula>VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Court 3 Player 2" dataDxfId="99"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Court 3 Lev Avg Dev" dataDxfId="98"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Court 3 Player 3" dataDxfId="97"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Court 3 Player 4" dataDxfId="96"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Gap1" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Court 3 Player 2" dataDxfId="106"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Court 3 Lev Avg Dev" dataDxfId="105"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Court 3 Player 3" dataDxfId="104"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Court 3 Player 4" dataDxfId="103"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Gap1" dataDxfId="102"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Gap2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Court 4 Week" dataDxfId="94"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Court 4 Match Date" dataDxfId="93">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Court 4 Week" dataDxfId="101"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Court 4 Match Date" dataDxfId="100">
       <calculatedColumnFormula>VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$58,11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Court 4 Player 1" dataDxfId="92">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Court 4 Player 1" dataDxfId="99">
       <calculatedColumnFormula>VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$58,12,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Court 4 Player 2" dataDxfId="91">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Court 4 Player 2" dataDxfId="98">
       <calculatedColumnFormula>VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$58,13,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Court 4 Lev Avg Dev" dataDxfId="90">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Court 4 Lev Avg Dev" dataDxfId="97">
       <calculatedColumnFormula>VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$58,14,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Court 4 Player 3" dataDxfId="89">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Court 4 Player 3" dataDxfId="96">
       <calculatedColumnFormula>VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$58,15,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Court 4 Player 4" dataDxfId="88">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Court 4 Player 4" dataDxfId="95">
       <calculatedColumnFormula>VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$58,16,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4CEAC13-27DC-4364-93F5-EF5E77F0FE7E}" name="Table22" displayName="Table22" ref="E4:E23" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
+  <autoFilter ref="E4:E23" xr:uid="{D4CEAC13-27DC-4364-93F5-EF5E77F0FE7E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E5:E19">
+    <sortCondition ref="E18:E33"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{337FB5BB-A8B5-4A9E-BD6A-CC64B3BE0B84}" name="NAME" dataDxfId="92"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2814,8 +2928,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:AJ59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18:R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2829,7 +2943,8 @@
     <col min="15" max="15" width="5" style="2" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" style="26" customWidth="1"/>
     <col min="17" max="17" width="4.7109375" style="27" customWidth="1"/>
-    <col min="18" max="19" width="4.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.28515625" style="2" customWidth="1"/>
     <col min="20" max="20" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.85546875" style="3" customWidth="1"/>
     <col min="22" max="23" width="13.85546875" style="1" customWidth="1"/>
@@ -3237,50 +3352,50 @@
       </c>
       <c r="U13" s="21">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,2,FALSE)</f>
-        <v>45960</v>
+        <v>46002</v>
       </c>
       <c r="V13" s="5" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,3,FALSE)</f>
-        <v>Goran Mecevic</v>
+        <v>Bob Alexander</v>
       </c>
       <c r="W13" s="5" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,4,FALSE)</f>
-        <v>Doug King</v>
+        <v>Claus Nussgruber</v>
       </c>
       <c r="X13" s="16">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,5,FALSE)</f>
-        <v>0.46875</v>
+        <v>0.375</v>
       </c>
       <c r="Y13" s="5" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,6,FALSE)</f>
-        <v>Norm Goldberg</v>
+        <v>Doug King</v>
       </c>
       <c r="Z13" s="5" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,7,FALSE)</f>
-        <v>Bill Tauriello</v>
+        <v>Norm Goldberg</v>
       </c>
       <c r="AC13" s="6" t="s">
         <v>25</v>
       </c>
       <c r="AD13" s="20">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,11,FALSE)</f>
-        <v>45960</v>
+        <v>46002</v>
       </c>
       <c r="AE13" s="14" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,12,FALSE)</f>
-        <v>Bill Taylor</v>
+        <v>Pierce Butler</v>
       </c>
       <c r="AF13" s="14" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,13,FALSE)</f>
-        <v>Claus Nussgruber</v>
+        <v>Serban Vasile</v>
       </c>
       <c r="AG13" s="4">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,14,FALSE)</f>
-        <v>0.25</v>
+        <v>0.1875</v>
       </c>
       <c r="AH13" s="14" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,15,FALSE)</f>
-        <v>Pierce Butler</v>
+        <v>Klaus Tum</v>
       </c>
       <c r="AI13" s="22" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY()),$T$19:$AI$59,16,FALSE)</f>
@@ -3293,54 +3408,54 @@
       </c>
       <c r="U14" s="21">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,2,FALSE)</f>
-        <v>45967</v>
+        <v>46009</v>
       </c>
       <c r="V14" s="5" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,3,FALSE)</f>
-        <v>Claus Nussgruber</v>
+        <v>Bill Tauriello</v>
       </c>
       <c r="W14" s="5" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,4,FALSE)</f>
-        <v>Bob Alexander</v>
+        <v>Bill Taylor</v>
       </c>
       <c r="X14" s="16">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,5,FALSE)</f>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="Y14" s="5" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,6,FALSE)</f>
-        <v>Bill Taylor</v>
+        <v>Claus Nussgruber</v>
       </c>
       <c r="Z14" s="5" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,7,FALSE)</f>
-        <v>Klaus Tum</v>
+        <v>Godehard Rau</v>
       </c>
       <c r="AC14" s="6" t="s">
         <v>26</v>
       </c>
       <c r="AD14" s="20">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,11,FALSE)</f>
-        <v>45967</v>
+        <v>46009</v>
       </c>
       <c r="AE14" s="14" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,12,FALSE)</f>
-        <v>Godehard Rau</v>
+        <v>Pierce Butler</v>
       </c>
       <c r="AF14" s="14" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,13,FALSE)</f>
-        <v>Bill Tauriello</v>
+        <v>Serban Vasile</v>
       </c>
       <c r="AG14" s="4">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,14,FALSE)</f>
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="AH14" s="14" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,15,FALSE)</f>
-        <v>Norm Goldberg</v>
+        <v>Goran Mecevic</v>
       </c>
       <c r="AI14" s="22" t="str">
         <f ca="1">VLOOKUP(WEEKNUM(TODAY())+1,$T$19:$AI$59,16,FALSE)</f>
-        <v>Doug King</v>
+        <v>Tom Powers</v>
       </c>
     </row>
     <row r="15" spans="20:36" x14ac:dyDescent="0.2">
@@ -3453,7 +3568,9 @@
       <c r="Q18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R18" s="1"/>
+      <c r="R18" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="S18" s="1"/>
       <c r="T18" s="16" t="s">
         <v>35</v>
@@ -3514,7 +3631,7 @@
       </c>
       <c r="K19" s="25">
         <f t="shared" ref="K19:K59" si="7">AVEDEV(VLOOKUP(F19,$M$19:$Q$37,5), VLOOKUP(G19,$M$19:$Q$37,5), VLOOKUP(H19,$M$19:$Q$37,5), VLOOKUP(I19,$M$19:$Q$37,5))</f>
-        <v>0.3125</v>
+        <v>0.21875</v>
       </c>
       <c r="M19" s="1">
         <v>1</v>
@@ -3531,7 +3648,9 @@
       <c r="Q19" s="1">
         <v>3</v>
       </c>
-      <c r="R19" s="1"/>
+      <c r="R19" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S19" s="1"/>
       <c r="T19" s="16">
         <f>WEEKNUM(U19)</f>
@@ -3579,7 +3698,7 @@
       </c>
       <c r="AG19" s="4">
         <f t="shared" ref="AG19:AG59" si="17">K19</f>
-        <v>0.3125</v>
+        <v>0.21875</v>
       </c>
       <c r="AH19" s="4" t="str">
         <f t="shared" ref="AH19:AH59" si="18">VLOOKUP(H19,$M$19:$N$41,2,FALSE) &amp; IF(ISERROR(SEARCH("~*",H19)),"","*")</f>
@@ -3624,7 +3743,7 @@
       </c>
       <c r="K20" s="25">
         <f t="shared" si="7"/>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="M20" s="1">
         <v>2</v>
@@ -3641,7 +3760,9 @@
       <c r="Q20" s="1">
         <v>3.5</v>
       </c>
-      <c r="R20" s="1"/>
+      <c r="R20" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S20" s="1"/>
       <c r="T20" s="16">
         <f t="shared" ref="T20:T57" si="20">WEEKNUM(U20)</f>
@@ -3689,7 +3810,7 @@
       </c>
       <c r="AG20" s="4">
         <f t="shared" si="17"/>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="AH20" s="4" t="str">
         <f t="shared" si="18"/>
@@ -3730,7 +3851,7 @@
       </c>
       <c r="J21" s="25">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="K21" s="25">
         <f t="shared" si="7"/>
@@ -3751,7 +3872,9 @@
       <c r="Q21" s="1">
         <v>3</v>
       </c>
-      <c r="R21" s="1"/>
+      <c r="R21" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S21" s="1"/>
       <c r="T21" s="16">
         <f t="shared" si="20"/>
@@ -3771,7 +3894,7 @@
       </c>
       <c r="X21" s="16">
         <f t="shared" si="11"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="Y21" s="16" t="str">
         <f t="shared" si="12"/>
@@ -3840,7 +3963,7 @@
       </c>
       <c r="J22" s="25">
         <f t="shared" si="6"/>
-        <v>0.1875</v>
+        <v>0</v>
       </c>
       <c r="K22" s="25">
         <f t="shared" si="7"/>
@@ -3861,7 +3984,9 @@
       <c r="Q22" s="1">
         <v>4</v>
       </c>
-      <c r="R22" s="1"/>
+      <c r="R22" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S22" s="1"/>
       <c r="T22" s="16">
         <f t="shared" si="20"/>
@@ -3881,7 +4006,7 @@
       </c>
       <c r="X22" s="16">
         <f t="shared" si="11"/>
-        <v>0.1875</v>
+        <v>0</v>
       </c>
       <c r="Y22" s="16" t="str">
         <f t="shared" si="12"/>
@@ -3971,7 +4096,9 @@
       <c r="Q23" s="1">
         <v>3</v>
       </c>
-      <c r="R23" s="1"/>
+      <c r="R23" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S23" s="1"/>
       <c r="T23" s="16">
         <f t="shared" si="20"/>
@@ -4081,7 +4208,9 @@
       <c r="Q24" s="1">
         <v>4</v>
       </c>
-      <c r="R24" s="1"/>
+      <c r="R24" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S24" s="1"/>
       <c r="T24" s="16">
         <f t="shared" si="20"/>
@@ -4191,7 +4320,9 @@
       <c r="Q25" s="1">
         <v>3</v>
       </c>
-      <c r="R25" s="1"/>
+      <c r="R25" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S25" s="1"/>
       <c r="T25" s="16">
         <f t="shared" si="20"/>
@@ -4301,7 +4432,9 @@
       <c r="Q26" s="1">
         <v>3.5</v>
       </c>
-      <c r="R26" s="1"/>
+      <c r="R26" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S26" s="1"/>
       <c r="T26" s="16">
         <f t="shared" si="20"/>
@@ -4411,7 +4544,9 @@
       <c r="Q27" s="1">
         <v>4</v>
       </c>
-      <c r="R27" s="1"/>
+      <c r="R27" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S27" s="1"/>
       <c r="T27" s="16">
         <f t="shared" si="20"/>
@@ -4500,7 +4635,7 @@
       </c>
       <c r="J28" s="25">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="K28" s="25">
         <f t="shared" si="7"/>
@@ -4521,7 +4656,9 @@
       <c r="Q28" s="1">
         <v>4.25</v>
       </c>
-      <c r="R28" s="1"/>
+      <c r="R28" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S28" s="1"/>
       <c r="T28" s="16">
         <f t="shared" si="20"/>
@@ -4541,7 +4678,7 @@
       </c>
       <c r="X28" s="16">
         <f t="shared" si="11"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="Y28" s="16" t="str">
         <f t="shared" si="12"/>
@@ -4631,7 +4768,9 @@
       <c r="Q29" s="1">
         <v>4</v>
       </c>
-      <c r="R29" s="1"/>
+      <c r="R29" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S29" s="1"/>
       <c r="T29" s="16">
         <f t="shared" si="20"/>
@@ -4724,7 +4863,7 @@
       </c>
       <c r="K30" s="25">
         <f t="shared" si="7"/>
-        <v>0.4375</v>
+        <v>0.40625</v>
       </c>
       <c r="M30" s="1">
         <v>12</v>
@@ -4739,9 +4878,11 @@
         <v>9083922379</v>
       </c>
       <c r="Q30" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="R30" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S30" s="1"/>
       <c r="T30" s="16">
         <f t="shared" si="20"/>
@@ -4789,7 +4930,7 @@
       </c>
       <c r="AG30" s="4">
         <f t="shared" si="17"/>
-        <v>0.4375</v>
+        <v>0.40625</v>
       </c>
       <c r="AH30" s="4" t="str">
         <f t="shared" si="18"/>
@@ -4851,7 +4992,9 @@
       <c r="Q31" s="1">
         <v>4</v>
       </c>
-      <c r="R31" s="1"/>
+      <c r="R31" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S31" s="1"/>
       <c r="T31" s="16">
         <f t="shared" si="20"/>
@@ -4961,7 +5104,9 @@
       <c r="Q32" s="1">
         <v>3.75</v>
       </c>
-      <c r="R32" s="1"/>
+      <c r="R32" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S32" s="1"/>
       <c r="T32" s="16">
         <f t="shared" si="20"/>
@@ -5054,7 +5199,7 @@
       </c>
       <c r="K33" s="25">
         <f t="shared" si="7"/>
-        <v>0.25</v>
+        <v>0.1875</v>
       </c>
       <c r="M33" s="1">
         <v>15</v>
@@ -5071,7 +5216,9 @@
       <c r="Q33" s="24">
         <v>4</v>
       </c>
-      <c r="R33" s="24"/>
+      <c r="R33" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="S33" s="1"/>
       <c r="T33" s="16">
         <f t="shared" si="20"/>
@@ -5119,7 +5266,7 @@
       </c>
       <c r="AG33" s="4">
         <f t="shared" si="17"/>
-        <v>0.25</v>
+        <v>0.1875</v>
       </c>
       <c r="AH33" s="4" t="str">
         <f t="shared" si="18"/>
@@ -5181,6 +5328,9 @@
       <c r="Q34" s="1">
         <v>3.75</v>
       </c>
+      <c r="R34" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="T34" s="16">
         <f t="shared" si="20"/>
         <v>51</v>
@@ -5289,6 +5439,9 @@
       <c r="Q35" s="1">
         <v>3.75</v>
       </c>
+      <c r="R35" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="T35" s="16">
         <f t="shared" si="20"/>
         <v>52</v>
@@ -5397,6 +5550,9 @@
       <c r="Q36" s="1">
         <v>3.75</v>
       </c>
+      <c r="R36" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="T36" s="16">
         <f t="shared" si="20"/>
         <v>1</v>
@@ -5505,6 +5661,9 @@
       <c r="Q37" s="1">
         <v>3.75</v>
       </c>
+      <c r="R37" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="T37" s="16">
         <f t="shared" si="20"/>
         <v>2</v>
@@ -5794,7 +5953,7 @@
       </c>
       <c r="K40" s="25">
         <f t="shared" si="7"/>
-        <v>0.4375</v>
+        <v>0.5625</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>58</v>
@@ -5848,7 +6007,7 @@
       </c>
       <c r="AG40" s="4">
         <f t="shared" si="17"/>
-        <v>0.4375</v>
+        <v>0.5625</v>
       </c>
       <c r="AH40" s="4" t="str">
         <f t="shared" si="18"/>
@@ -5992,7 +6151,7 @@
       </c>
       <c r="K42" s="25">
         <f t="shared" si="7"/>
-        <v>0.4375</v>
+        <v>0.40625</v>
       </c>
       <c r="T42" s="16">
         <f t="shared" si="20"/>
@@ -6040,7 +6199,7 @@
       </c>
       <c r="AG42" s="4">
         <f t="shared" si="17"/>
-        <v>0.4375</v>
+        <v>0.40625</v>
       </c>
       <c r="AH42" s="4" t="str">
         <f t="shared" si="18"/>
@@ -6457,7 +6616,7 @@
       </c>
       <c r="K47" s="25">
         <f t="shared" si="7"/>
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="T47" s="16">
         <f t="shared" si="20"/>
@@ -6505,7 +6664,7 @@
       </c>
       <c r="AG47" s="4">
         <f t="shared" si="17"/>
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="AH47" s="4" t="str">
         <f t="shared" si="18"/>
@@ -6736,7 +6895,7 @@
       </c>
       <c r="K50" s="25">
         <f t="shared" si="7"/>
-        <v>0.4375</v>
+        <v>0.40625</v>
       </c>
       <c r="T50" s="16">
         <f t="shared" si="20"/>
@@ -6784,7 +6943,7 @@
       </c>
       <c r="AG50" s="4">
         <f t="shared" si="17"/>
-        <v>0.4375</v>
+        <v>0.40625</v>
       </c>
       <c r="AH50" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7011,7 +7170,7 @@
       </c>
       <c r="J53" s="25">
         <f t="shared" si="6"/>
-        <v>0.4375</v>
+        <v>0.40625</v>
       </c>
       <c r="K53" s="25">
         <f t="shared" si="7"/>
@@ -7035,7 +7194,7 @@
       </c>
       <c r="X53" s="16">
         <f t="shared" si="11"/>
-        <v>0.4375</v>
+        <v>0.40625</v>
       </c>
       <c r="Y53" s="16" t="str">
         <f t="shared" si="12"/>
@@ -7108,7 +7267,7 @@
       </c>
       <c r="K54" s="25">
         <f t="shared" si="7"/>
-        <v>0.3125</v>
+        <v>0.34375</v>
       </c>
       <c r="T54" s="16">
         <f t="shared" si="20"/>
@@ -7156,7 +7315,7 @@
       </c>
       <c r="AG54" s="4">
         <f t="shared" si="17"/>
-        <v>0.3125</v>
+        <v>0.34375</v>
       </c>
       <c r="AH54" s="4" t="str">
         <f t="shared" si="18"/>
@@ -7197,7 +7356,7 @@
       </c>
       <c r="J55" s="25">
         <f t="shared" si="6"/>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="K55" s="25">
         <f t="shared" si="7"/>
@@ -7221,7 +7380,7 @@
       </c>
       <c r="X55" s="16">
         <f t="shared" si="11"/>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="Y55" s="16" t="str">
         <f t="shared" si="12"/>
@@ -7290,7 +7449,7 @@
       </c>
       <c r="J56" s="25">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="K56" s="25">
         <f t="shared" si="7"/>
@@ -7314,7 +7473,7 @@
       </c>
       <c r="X56" s="16">
         <f t="shared" si="11"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="Y56" s="16" t="str">
         <f t="shared" si="12"/>
@@ -7643,145 +7802,157 @@
     <mergeCell ref="AD18:AI18"/>
   </mergeCells>
   <conditionalFormatting sqref="T16:Z16">
-    <cfRule type="timePeriod" dxfId="77" priority="120" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="81" priority="120" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(T16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(T16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="76" priority="121" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="80" priority="121" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(T16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(T16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576 AD11:AD1048576 AC7:AC10 AD2:AD6">
-    <cfRule type="cellIs" dxfId="75" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="170" operator="equal">
       <formula>$U$16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14">
-    <cfRule type="timePeriod" dxfId="74" priority="160" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="78" priority="160" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(U14,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(U14,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="73" priority="161" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="77" priority="161" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(U14,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(U14,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U13:Z13 V14:Z14">
-    <cfRule type="timePeriod" dxfId="72" priority="163" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="76" priority="162" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(U13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(U13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="75" priority="163" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(U13,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(U13,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="71" priority="162" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(U13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(U13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U19:Z19 V19:Z59 U20:U59">
-    <cfRule type="timePeriod" dxfId="70" priority="167" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="74" priority="165" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(U19,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(U19,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="73" priority="167" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(U19,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(U19,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="69" priority="165" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(U19,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(U19,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W39:W59">
-    <cfRule type="timePeriod" dxfId="65" priority="22" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="69" priority="22" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(W39,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(W39,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="64" priority="23" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="68" priority="23" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(W39,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(W39,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:X14">
-    <cfRule type="timePeriod" dxfId="61" priority="1" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="65" priority="1" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(X12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(X12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="60" priority="2" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="64" priority="2" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(X12,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(X12,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y39:Z59">
-    <cfRule type="timePeriod" dxfId="58" priority="14" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="61" priority="14" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(Y39,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(Y39,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="56" priority="15" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="60" priority="15" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(Y39,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(Y39,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC16">
-    <cfRule type="timePeriod" dxfId="51" priority="112" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="55" priority="109" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(AC16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AC16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="54" priority="110" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AC16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AC16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="50" priority="109" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="53" priority="111" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AC16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AC16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="49" priority="111" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(AC16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AC16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="48" priority="110" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="52" priority="112" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AC16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AC16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC16:AI16">
-    <cfRule type="timePeriod" dxfId="47" priority="114" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="51" priority="105" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(AC16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AC16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="50" priority="106" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AC16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AC16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="46" priority="113" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="49" priority="113" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AC16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AC16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="45" priority="106" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="48" priority="114" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AC16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AC16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="44" priority="105" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(AC16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AC16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD14 AD16:AI16">
-    <cfRule type="timePeriod" dxfId="43" priority="155" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="47" priority="152" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(AD14,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD14,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="46" priority="155" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AD14,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD14,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="42" priority="156" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(AD14,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD14,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="41" priority="152" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="45" priority="156" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AD14,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD14,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD16">
-    <cfRule type="timePeriod" dxfId="40" priority="94" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="44" priority="86" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(AD16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="43" priority="87" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AD16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="39" priority="86" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="42" priority="93" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AD16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="38" priority="87" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="41" priority="94" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AD16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="37" priority="93" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(AD16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD13:AE14 AD13:AI13 AE14:AI14">
-    <cfRule type="timePeriod" dxfId="36" priority="157" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="40" priority="153" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AD13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="35" priority="153" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="39" priority="157" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AD13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD13:AI13 AD13:AE14 AE14:AI14">
-    <cfRule type="timePeriod" dxfId="34" priority="154" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="38" priority="154" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AD13,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD13,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="33" priority="158" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="37" priority="158" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AD13,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD13,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD16:AI16 AD14">
-    <cfRule type="timePeriod" dxfId="32" priority="151" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="36" priority="151" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AD14,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD14,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD16:AI16">
-    <cfRule type="timePeriod" dxfId="31" priority="97" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="35" priority="97" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AD16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="30" priority="100" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="34" priority="98" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(AD16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="33" priority="99" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(AD16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="32" priority="100" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(AD16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="31" priority="103" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(AD16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="30" priority="104" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AD16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
     <cfRule type="timePeriod" dxfId="29" priority="118" timePeriod="nextWeek">
@@ -7790,88 +7961,76 @@
     <cfRule type="timePeriod" dxfId="28" priority="119" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AD16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="27" priority="103" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(AD16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="26" priority="104" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(AD16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="25" priority="99" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(AD16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="24" priority="98" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(AD16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD19:AI59">
-    <cfRule type="timePeriod" dxfId="23" priority="164" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="27" priority="164" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AD19,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AD19,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="22" priority="166" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="26" priority="166" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AD19,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AD19,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE19:AI59">
-    <cfRule type="timePeriod" dxfId="21" priority="145" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="25" priority="145" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AE19,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AE19,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="20" priority="146" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="24" priority="146" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AE19,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AE19,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG12">
-    <cfRule type="timePeriod" dxfId="18" priority="50" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="22" priority="49" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(AG12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AG12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="21" priority="50" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AG12,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AG12,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="17" priority="51" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="20" priority="51" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AG12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AG12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="15" priority="54" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="19" priority="52" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AG12,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AG12,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="14" priority="52" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(AG12,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AG12,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="13" priority="53" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="18" priority="53" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AG12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AG12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="12" priority="49" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(AG12,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AG12,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    <cfRule type="timePeriod" dxfId="17" priority="54" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(AG12,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AG12,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG13:AG14">
-    <cfRule type="timePeriod" dxfId="11" priority="149" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="15" priority="149" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AG13,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AG13,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="10" priority="150" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="14" priority="150" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AG13,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AG13,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG16">
-    <cfRule type="timePeriod" dxfId="9" priority="101" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="13" priority="95" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AG16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AG16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="8" priority="102" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="12" priority="96" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AG16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AG16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="7" priority="95" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="11" priority="101" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AG16,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AG16,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="6" priority="96" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="10" priority="102" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AG16,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AG16,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH19:AI59">
-    <cfRule type="timePeriod" dxfId="4" priority="134" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="8" priority="133" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(AH19,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AH19,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="7" priority="134" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AH19,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AH19,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="3" priority="133" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="6" priority="137" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(AH19,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AH19,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="2" priority="137" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(AH19,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(AH19,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
-    </cfRule>
-    <cfRule type="timePeriod" dxfId="1" priority="138" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="5" priority="138" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(AH19,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(AH19,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7925,11 +8084,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A11:XFD17 V19:Z59 A18:B18 F18 J18:M18 S18:XFD19 N18:N37 B19:C20 H19:M20 D19:G30 AE19:AI59 S20:U20 J20:K59 AA20:XFD59 H21:L29 S21:T33 M21:M37 U21:U57 H30:I30 J30:L59 I31 N34:S36 O34:T57 M38:N41 M42:S1048576 T58:U58 O59:U59 A60:L1048576 O60:XFD1048576 A19:A59</xm:sqref>
+          <xm:sqref>A11:XFD17 V19:Z59 A18:B18 F18 J18:M18 S18:XFD19 N18:N37 H19:M20 A19:A59 AE19:AI59 S20:U20 J20:K59 AA20:XFD59 H21:L29 M21:M37 U21:U57 H30:I30 J30:L59 I31 N34:Q36 O38:T57 M38:N41 M42:S1048576 T58:U58 O59:U59 A60:L1048576 O60:XFD1048576 O34:Q37 S21:T37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="32" operator="containsText" id="{0FA8A02A-6CFE-43F4-B22E-AD821B16B6AD}">
-            <xm:f>NOT(ISERROR(SEARCH($X$2,B21)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($X$2,B19)))</xm:f>
             <xm:f>$X$2</xm:f>
             <x14:dxf>
               <font>
@@ -7943,7 +8102,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="33" operator="containsText" id="{E4D3AD1A-F59D-4AC2-A888-3CBB1F0D32BC}">
-            <xm:f>NOT(ISERROR(SEARCH($U$2,B21)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($U$2,B19)))</xm:f>
             <xm:f>$U$2</xm:f>
             <x14:dxf>
               <font>
@@ -7956,7 +8115,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B21:C30</xm:sqref>
+          <xm:sqref>B19:G30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="11" operator="containsText" id="{7C7D81E0-5452-4C36-8734-2D3A6279487C}">
@@ -8018,7 +8177,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>O18:R33</xm:sqref>
+          <xm:sqref>O18:R19 O20:Q33 R20:R37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="169" operator="containsText" id="{D8BFC164-F5A8-484A-B7BF-6FE26714466A}">
@@ -8035,7 +8194,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>S18:Z19 V19:Z59 S20:U20 U21:U57 T58:U59 O59:U59 AC19:XFD59 N13:Z14 AC13:AI14 AD16:XFD17 N16:Z17 N12:V12 AD12:AE12 AJ12:XFD15 A12:M17 N15:T15 A18:B18 F18 J18:M18 AC18:AD18 AJ18:XFD18 N18:N37 B19:C20 H19:M20 D19:G30 J20:K59 H21:L29 S21:T33 M21:M37 H30:I30 J30:L59 I31 N34:S36 O34:T57 M38:N41 M42:S1048576 AA59 A60:L1048576 O60:AA1048576 AD60:XFD1048576 T2:U5 A19:A59</xm:sqref>
+          <xm:sqref>S18:Z19 V19:Z59 S20:U20 U21:U57 T58:U59 O59:U59 AC19:XFD59 N13:Z14 AC13:AI14 AD16:XFD17 N16:Z17 N12:V12 AD12:AE12 AJ12:XFD15 A12:M17 N15:T15 A18:B18 F18 J18:M18 AC18:AD18 AJ18:XFD18 N18:N37 H19:M20 A19:A59 J20:K59 H21:L29 M21:M37 H30:I30 J30:L59 I31 N34:Q36 O38:T57 M38:N41 M42:S1048576 AA59 A60:L1048576 O60:AA1048576 AD60:XFD1048576 T2:U5 O34:Q37 S21:T37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="92" operator="containsText" id="{E9B17E93-9CFB-473E-A999-03215258D456}">
@@ -8154,6 +8313,20 @@
           <xm:sqref>Y12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{77A2D7F2-FCB2-427C-9818-56AF99DBB9BF}">
+            <xm:f>NOT(ISERROR(SEARCH($X$2,Y39)))</xm:f>
+            <xm:f>$X$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF6600FF"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCCCCFF"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="containsText" priority="16" operator="containsText" id="{CF870D08-E172-4396-AC9F-264DFDA29933}">
             <xm:f>NOT(ISERROR(SEARCH($U$2,Y39)))</xm:f>
             <xm:f>$U$2</xm:f>
@@ -8164,20 +8337,6 @@
               <fill>
                 <patternFill>
                   <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{77A2D7F2-FCB2-427C-9818-56AF99DBB9BF}">
-            <xm:f>NOT(ISERROR(SEARCH($X$2,Y39)))</xm:f>
-            <xm:f>$X$2</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF6600FF"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFCCCCFF"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -8307,4 +8466,497 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563664C2-B597-4B0F-B2D5-B86AD58B3EB3}">
+  <dimension ref="D4:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="27">
+        <v>9083042902</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="27">
+        <v>9082172116</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="27">
+        <v>9085077500</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="27">
+        <v>9085774273</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="27">
+        <v>9085863385</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="27">
+        <v>9088720433</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="1">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="27">
+        <v>9082687951</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="27">
+        <v>9085004213</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D13" s="1">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="27">
+        <v>9085287696</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="27">
+        <v>9086194475</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="27">
+        <v>9088924833</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="1">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="27">
+        <v>9083922379</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="27">
+        <v>9086255023</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D18" s="1">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="27">
+        <v>9083297532</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D19" s="1">
+        <v>15</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="28">
+        <v>9088122100</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="24">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D20" s="1">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="26">
+        <v>9083100187</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D21" s="1">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="26">
+        <v>9085077440</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D22" s="1">
+        <v>18</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="26">
+        <v>9088928428</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D23" s="1">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="26">
+        <v>9083031793</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{F79F8E31-41BD-4901-A11F-FE32E103C712}">
+            <xm:f>NOT(ISERROR(SEARCH($X$2,D4)))</xm:f>
+            <xm:f>$X$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF6600FF"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCCCCFF"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D4:E23 F20:H23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{9609ABDB-3095-40F4-AE0C-8891A280197A}">
+            <xm:f>NOT(ISERROR(SEARCH($X$2,F4)))</xm:f>
+            <xm:f>$X$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF6600FF"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCCCCFF"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{B5E09111-999C-458D-985E-F82692153A81}">
+            <xm:f>NOT(ISERROR(SEARCH($U$2,F4)))</xm:f>
+            <xm:f>$U$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I6:I23 F4:I5 F6:H19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{26AD4612-9BA5-46C7-BF15-5643444700BD}">
+            <xm:f>NOT(ISERROR(SEARCH($U$2,D4)))</xm:f>
+            <xm:f>$U$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D4:E23 F20:H23</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>